<commit_message>
Updated data labels on graphs
Updated data labels and added categories for values
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LucanSinclair\OneDrive - Earthwatch\Desktop\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LucanSinclair\OneDrive - Earthwatch\Desktop\Code\Earthwatch_Code\Saltmarsh-Savers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483F4A55-C3A9-43FF-B9D5-BB86511F629F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB90DB66-54C7-4263-A117-97443DC0CB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="3830" windowWidth="14400" windowHeight="8170" activeTab="1" xr2:uid="{0EAD53D3-40C8-4F45-90C6-CC9001D417E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{0EAD53D3-40C8-4F45-90C6-CC9001D417E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Category</t>
   </si>
@@ -187,6 +187,24 @@
   </si>
   <si>
     <t>Climate</t>
+  </si>
+  <si>
+    <t>Fish Habitat</t>
+  </si>
+  <si>
+    <t>Carbon Storage</t>
+  </si>
+  <si>
+    <t>Water Quality</t>
+  </si>
+  <si>
+    <t>Habitat Values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recreation </t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -329,7 +347,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,6 +525,42 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -670,8 +724,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1047,204 +1107,248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4EEEF6-3C44-4420-920E-6CE8C12FABCF}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" customWidth="1"/>
+    <col min="9" max="9" width="22.6328125" customWidth="1"/>
+    <col min="10" max="10" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2">
+        <v>21.352985638699927</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5.8956916099773249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>15.457294028722602</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5.7067271352985633</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>23.80952380952381</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3.8926681783824644</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5">
+        <v>21.012849584278158</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3.5525321239606953</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6">
+        <v>7.2184429327286477</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2.3053665910808774</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7">
+        <v>11.148904006046862</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
+      <c r="D7" s="2">
         <v>6.0090702947845802</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5.291005291005292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4.157218442932729</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5.7823129251700678</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5.5555555555555562</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3">
+        <v>4.1194255479969764</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3">
+        <v>3.7414965986394559</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2.7588813303099018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1.8518518518518516</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3">
+      <c r="D16" s="4">
         <v>5.9334845049130776</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>5.8956916099773249</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>5.7823129251700678</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>5.7067271352985633</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="4">
+        <v>5.4043839758125474</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5.1020408163265305</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="4">
+        <v>4.5729402872260012</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="5">
+        <v>5.291005291005292</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1.9274376417233559</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B7">
+      <c r="D22" s="6">
         <v>5.6311413454270607</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>5.5555555555555562</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B9">
+      <c r="D23" s="6">
         <v>5.5177626606198027</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10">
-        <v>5.4043839758125474</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>5.291005291005292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12">
-        <v>5.291005291005292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13">
-        <v>5.1020408163265305</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>4.5729402872260012</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15">
-        <v>4.157218442932729</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16">
-        <v>4.1194255479969764</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>3.8926681783824644</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18">
-        <v>3.7414965986394559</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19">
-        <v>3.5525321239606953</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20">
-        <v>2.7588813303099018</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>2.3053665910808774</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>1.9274376417233559</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23">
-        <v>1.8518518518518516</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B23">
-    <sortCondition descending="1" ref="B2:B23"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C20:D21">
+    <sortCondition descending="1" ref="D20:D21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1254,7 +1358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1045FBD-1EA5-4649-83FB-FF074C60F7A6}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>